<commit_message>
Test new billing policy
</commit_message>
<xml_diff>
--- a/tests/resources/mock_user_form.xlsx
+++ b/tests/resources/mock_user_form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -128,6 +128,24 @@
   </si>
   <si>
     <t xml:space="preserve">Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppomegranate@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomegranate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qquince@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quentin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quince</t>
   </si>
 </sst>
 </file>
@@ -274,10 +292,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="21.5"/>
   </cols>
@@ -467,22 +485,50 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="4" t="n">
+        <v>44119.5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>44211</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="4" t="n">
+        <v>44208.5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>44439</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
@@ -917,6 +963,8 @@
     <hyperlink ref="B6" r:id="rId5" display="llemon@example.com"/>
     <hyperlink ref="B7" r:id="rId6" display="nnectarine@example.com"/>
     <hyperlink ref="B8" r:id="rId7" display="oorange@example.com"/>
+    <hyperlink ref="B9" r:id="rId8" display="ppomegranate@example.com"/>
+    <hyperlink ref="B10" r:id="rId9" display="qquince@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fix formatting disconnects with Google Forms
</commit_message>
<xml_diff>
--- a/tests/resources/mock_user_form.xlsx
+++ b/tests/resources/mock_user_form.xlsx
@@ -34,13 +34,13 @@
     <t xml:space="preserve">Last name</t>
   </si>
   <si>
-    <t xml:space="preserve">PI Name</t>
+    <t xml:space="preserve">PI Last Name</t>
   </si>
   <si>
     <t xml:space="preserve">Contract end date (account expiration)</t>
   </si>
   <si>
-    <t xml:space="preserve">Do you need your account to be a power user account? (There is a fee associated with power user accounts.  Check with your PI first!)</t>
+    <t xml:space="preserve">Do you need your account to be a power user account?</t>
   </si>
   <si>
     <t xml:space="preserve">eelderberry@example.com</t>
@@ -331,10 +331,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="21.5"/>
   </cols>

</xml_diff>

<commit_message>
Update handling of account reactivation
</commit_message>
<xml_diff>
--- a/tests/resources/mock_user_form.xlsx
+++ b/tests/resources/mock_user_form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t xml:space="preserve">Vanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxigua@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xavier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xigua</t>
   </si>
 </sst>
 </file>
@@ -331,10 +340,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="21.5"/>
   </cols>
@@ -662,13 +671,27 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="4" t="n">
+        <v>43749.4583333333</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>43889</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
@@ -1064,10 +1087,11 @@
     <hyperlink ref="B12" r:id="rId11" display="ttomato@example.com"/>
     <hyperlink ref="B13" r:id="rId12" display="uugni@example.com"/>
     <hyperlink ref="B14" r:id="rId13" display="vvanilla@example.com"/>
+    <hyperlink ref="B15" r:id="rId14" display="xxigua@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>